<commit_message>
react front, flask back, fucked-up CORS
</commit_message>
<xml_diff>
--- a/yudhistira-back/menu_data.xlsx
+++ b/yudhistira-back/menu_data.xlsx
@@ -404,7 +404,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -419,12 +419,6 @@
       <sz val="15"/>
       <color indexed="8"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Times Roman"/>
     </font>
     <font>
       <sz val="12"/>
@@ -565,7 +559,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -573,49 +567,31 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1668,7 +1644,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1681,7 +1657,7 @@
     <col min="6" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.55" customHeight="1">
+    <row r="1" ht="16.5" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
@@ -1698,7 +1674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="30.55" customHeight="1">
+    <row r="2" ht="30.6" customHeight="1">
       <c r="A2" t="s" s="3">
         <v>5</v>
       </c>
@@ -1711,9 +1687,11 @@
       <c r="D2" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" ht="44.35" customHeight="1">
+      <c r="E2" s="6">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="3" ht="44.45" customHeight="1">
       <c r="A3" t="s" s="7">
         <v>9</v>
       </c>
@@ -1726,9 +1704,11 @@
       <c r="D3" t="s" s="9">
         <v>11</v>
       </c>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" ht="44.35" customHeight="1">
+      <c r="E3" s="10">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="4" ht="44.45" customHeight="1">
       <c r="A4" t="s" s="7">
         <v>12</v>
       </c>
@@ -1741,9 +1721,11 @@
       <c r="D4" t="s" s="9">
         <v>14</v>
       </c>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" ht="44.35" customHeight="1">
+      <c r="E4" s="10">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="5" ht="44.45" customHeight="1">
       <c r="A5" t="s" s="7">
         <v>15</v>
       </c>
@@ -1756,7 +1738,9 @@
       <c r="D5" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="10">
+        <v>20000</v>
+      </c>
     </row>
     <row r="6" ht="58.35" customHeight="1">
       <c r="A6" t="s" s="7">
@@ -1771,7 +1755,9 @@
       <c r="D6" t="s" s="9">
         <v>20</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="10">
+        <v>22000</v>
+      </c>
     </row>
     <row r="7" ht="58.35" customHeight="1">
       <c r="A7" t="s" s="7">
@@ -1786,9 +1772,11 @@
       <c r="D7" t="s" s="9">
         <v>23</v>
       </c>
-      <c r="E7" s="10"/>
-    </row>
-    <row r="8" ht="44.35" customHeight="1">
+      <c r="E7" s="10">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="8" ht="44.45" customHeight="1">
       <c r="A8" t="s" s="7">
         <v>24</v>
       </c>
@@ -1801,9 +1789,11 @@
       <c r="D8" t="s" s="9">
         <v>26</v>
       </c>
-      <c r="E8" s="10"/>
-    </row>
-    <row r="9" ht="44.35" customHeight="1">
+      <c r="E8" s="10">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="9" ht="44.45" customHeight="1">
       <c r="A9" t="s" s="7">
         <v>27</v>
       </c>
@@ -1816,9 +1806,11 @@
       <c r="D9" t="s" s="9">
         <v>29</v>
       </c>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" ht="44.35" customHeight="1">
+      <c r="E9" s="10">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="10" ht="44.45" customHeight="1">
       <c r="A10" t="s" s="7">
         <v>30</v>
       </c>
@@ -1831,9 +1823,11 @@
       <c r="D10" t="s" s="9">
         <v>33</v>
       </c>
-      <c r="E10" s="10"/>
-    </row>
-    <row r="11" ht="44.35" customHeight="1">
+      <c r="E10" s="10">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="11" ht="44.45" customHeight="1">
       <c r="A11" t="s" s="7">
         <v>34</v>
       </c>
@@ -1846,9 +1840,11 @@
       <c r="D11" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="E11" s="10"/>
-    </row>
-    <row r="12" ht="44.35" customHeight="1">
+      <c r="E11" s="10">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="12" ht="44.45" customHeight="1">
       <c r="A12" t="s" s="7">
         <v>37</v>
       </c>
@@ -1861,9 +1857,11 @@
       <c r="D12" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="E12" s="10"/>
-    </row>
-    <row r="13" ht="44.35" customHeight="1">
+      <c r="E12" s="10">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="13" ht="44.45" customHeight="1">
       <c r="A13" t="s" s="7">
         <v>40</v>
       </c>
@@ -1876,9 +1874,11 @@
       <c r="D13" t="s" s="9">
         <v>42</v>
       </c>
-      <c r="E13" s="10"/>
-    </row>
-    <row r="14" ht="44.35" customHeight="1">
+      <c r="E13" s="10">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="14" ht="44.45" customHeight="1">
       <c r="A14" t="s" s="7">
         <v>43</v>
       </c>
@@ -1891,9 +1891,11 @@
       <c r="D14" t="s" s="9">
         <v>45</v>
       </c>
-      <c r="E14" s="10"/>
-    </row>
-    <row r="15" ht="44.35" customHeight="1">
+      <c r="E14" s="10">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="15" ht="44.45" customHeight="1">
       <c r="A15" t="s" s="7">
         <v>46</v>
       </c>
@@ -1906,9 +1908,11 @@
       <c r="D15" t="s" s="9">
         <v>49</v>
       </c>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" ht="44.35" customHeight="1">
+      <c r="E15" s="10">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="16" ht="44.45" customHeight="1">
       <c r="A16" t="s" s="7">
         <v>50</v>
       </c>
@@ -1921,9 +1925,11 @@
       <c r="D16" t="s" s="9">
         <v>52</v>
       </c>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" ht="44.35" customHeight="1">
+      <c r="E16" s="10">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="17" ht="44.45" customHeight="1">
       <c r="A17" t="s" s="7">
         <v>53</v>
       </c>
@@ -1936,9 +1942,11 @@
       <c r="D17" t="s" s="9">
         <v>55</v>
       </c>
-      <c r="E17" s="10"/>
-    </row>
-    <row r="18" ht="44.35" customHeight="1">
+      <c r="E17" s="10">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="18" ht="44.45" customHeight="1">
       <c r="A18" t="s" s="7">
         <v>56</v>
       </c>
@@ -1951,9 +1959,11 @@
       <c r="D18" t="s" s="9">
         <v>58</v>
       </c>
-      <c r="E18" s="10"/>
-    </row>
-    <row r="19" ht="44.35" customHeight="1">
+      <c r="E18" s="10">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="19" ht="44.45" customHeight="1">
       <c r="A19" t="s" s="7">
         <v>59</v>
       </c>
@@ -1966,9 +1976,11 @@
       <c r="D19" t="s" s="9">
         <v>61</v>
       </c>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" ht="44.35" customHeight="1">
+      <c r="E19" s="10">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="20" ht="44.45" customHeight="1">
       <c r="A20" t="s" s="7">
         <v>62</v>
       </c>
@@ -1981,9 +1993,11 @@
       <c r="D20" t="s" s="9">
         <v>64</v>
       </c>
-      <c r="E20" s="10"/>
-    </row>
-    <row r="21" ht="44.35" customHeight="1">
+      <c r="E20" s="10">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="21" ht="44.45" customHeight="1">
       <c r="A21" t="s" s="7">
         <v>65</v>
       </c>
@@ -1996,9 +2010,11 @@
       <c r="D21" t="s" s="9">
         <v>67</v>
       </c>
-      <c r="E21" s="10"/>
-    </row>
-    <row r="22" ht="44.35" customHeight="1">
+      <c r="E21" s="10">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="22" ht="44.45" customHeight="1">
       <c r="A22" t="s" s="7">
         <v>68</v>
       </c>
@@ -2011,9 +2027,11 @@
       <c r="D22" t="s" s="9">
         <v>71</v>
       </c>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" ht="44.35" customHeight="1">
+      <c r="E22" s="10">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="23" ht="44.45" customHeight="1">
       <c r="A23" t="s" s="7">
         <v>72</v>
       </c>
@@ -2026,9 +2044,11 @@
       <c r="D23" t="s" s="9">
         <v>74</v>
       </c>
-      <c r="E23" s="10"/>
-    </row>
-    <row r="24" ht="44.35" customHeight="1">
+      <c r="E23" s="10">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="24" ht="44.45" customHeight="1">
       <c r="A24" t="s" s="7">
         <v>75</v>
       </c>
@@ -2041,9 +2061,11 @@
       <c r="D24" t="s" s="9">
         <v>77</v>
       </c>
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" ht="44.35" customHeight="1">
+      <c r="E24" s="10">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="25" ht="44.45" customHeight="1">
       <c r="A25" t="s" s="7">
         <v>78</v>
       </c>
@@ -2056,9 +2078,11 @@
       <c r="D25" t="s" s="9">
         <v>80</v>
       </c>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" ht="44.35" customHeight="1">
+      <c r="E25" s="10">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="26" ht="44.45" customHeight="1">
       <c r="A26" t="s" s="7">
         <v>81</v>
       </c>
@@ -2071,9 +2095,11 @@
       <c r="D26" t="s" s="9">
         <v>84</v>
       </c>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" ht="44.35" customHeight="1">
+      <c r="E26" s="10">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="27" ht="44.45" customHeight="1">
       <c r="A27" t="s" s="7">
         <v>85</v>
       </c>
@@ -2086,9 +2112,11 @@
       <c r="D27" t="s" s="9">
         <v>87</v>
       </c>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" ht="44.35" customHeight="1">
+      <c r="E27" s="10">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="28" ht="44.45" customHeight="1">
       <c r="A28" t="s" s="7">
         <v>88</v>
       </c>
@@ -2101,9 +2129,11 @@
       <c r="D28" t="s" s="9">
         <v>90</v>
       </c>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" ht="44.35" customHeight="1">
+      <c r="E28" s="10">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="29" ht="44.45" customHeight="1">
       <c r="A29" t="s" s="7">
         <v>91</v>
       </c>
@@ -2116,9 +2146,11 @@
       <c r="D29" t="s" s="9">
         <v>93</v>
       </c>
-      <c r="E29" s="10"/>
-    </row>
-    <row r="30" ht="44.35" customHeight="1">
+      <c r="E29" s="10">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="30" ht="44.45" customHeight="1">
       <c r="A30" t="s" s="7">
         <v>94</v>
       </c>
@@ -2131,9 +2163,11 @@
       <c r="D30" t="s" s="9">
         <v>96</v>
       </c>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" ht="44.35" customHeight="1">
+      <c r="E30" s="10">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="31" ht="44.45" customHeight="1">
       <c r="A31" t="s" s="7">
         <v>97</v>
       </c>
@@ -2146,9 +2180,11 @@
       <c r="D31" t="s" s="9">
         <v>99</v>
       </c>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" ht="44.35" customHeight="1">
+      <c r="E31" s="10">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="32" ht="44.45" customHeight="1">
       <c r="A32" t="s" s="7">
         <v>100</v>
       </c>
@@ -2161,9 +2197,11 @@
       <c r="D32" t="s" s="9">
         <v>102</v>
       </c>
-      <c r="E32" s="10"/>
-    </row>
-    <row r="33" ht="44.35" customHeight="1">
+      <c r="E32" s="10">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="33" ht="44.45" customHeight="1">
       <c r="A33" t="s" s="7">
         <v>103</v>
       </c>
@@ -2176,9 +2214,11 @@
       <c r="D33" t="s" s="9">
         <v>106</v>
       </c>
-      <c r="E33" s="10"/>
-    </row>
-    <row r="34" ht="44.35" customHeight="1">
+      <c r="E33" s="10">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="34" ht="44.45" customHeight="1">
       <c r="A34" t="s" s="7">
         <v>107</v>
       </c>
@@ -2191,9 +2231,11 @@
       <c r="D34" t="s" s="9">
         <v>109</v>
       </c>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" ht="44.35" customHeight="1">
+      <c r="E34" s="10">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="35" ht="44.45" customHeight="1">
       <c r="A35" t="s" s="7">
         <v>110</v>
       </c>
@@ -2206,9 +2248,11 @@
       <c r="D35" t="s" s="9">
         <v>112</v>
       </c>
-      <c r="E35" s="10"/>
-    </row>
-    <row r="36" ht="30.35" customHeight="1">
+      <c r="E35" s="10">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="36" ht="30.4" customHeight="1">
       <c r="A36" t="s" s="7">
         <v>113</v>
       </c>
@@ -2221,9 +2265,11 @@
       <c r="D36" t="s" s="9">
         <v>115</v>
       </c>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" ht="44.35" customHeight="1">
+      <c r="E36" s="10">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="37" ht="44.45" customHeight="1">
       <c r="A37" t="s" s="7">
         <v>116</v>
       </c>
@@ -2236,7 +2282,9 @@
       <c r="D37" t="s" s="9">
         <v>118</v>
       </c>
-      <c r="E37" s="10"/>
+      <c r="E37" s="10">
+        <v>22000</v>
+      </c>
     </row>
     <row r="38" ht="58.35" customHeight="1">
       <c r="A38" t="s" s="7">
@@ -2251,9 +2299,11 @@
       <c r="D38" t="s" s="9">
         <v>121</v>
       </c>
-      <c r="E38" s="10"/>
-    </row>
-    <row r="39" ht="30.35" customHeight="1">
+      <c r="E38" s="10">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="39" ht="30.4" customHeight="1">
       <c r="A39" t="s" s="7">
         <v>122</v>
       </c>
@@ -2266,9 +2316,11 @@
       <c r="D39" t="s" s="9">
         <v>124</v>
       </c>
-      <c r="E39" s="10"/>
-    </row>
-    <row r="40" ht="44.35" customHeight="1">
+      <c r="E39" s="10">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="40" ht="44.45" customHeight="1">
       <c r="A40" t="s" s="7">
         <v>125</v>
       </c>
@@ -2281,49 +2333,9 @@
       <c r="D40" t="s" s="9">
         <v>127</v>
       </c>
-      <c r="E40" s="10"/>
-    </row>
-    <row r="41" ht="16.35" customHeight="1">
-      <c r="A41" s="11"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-    </row>
-    <row r="42" ht="16.35" customHeight="1">
-      <c r="A42" s="14"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="10"/>
-    </row>
-    <row r="43" ht="16.35" customHeight="1">
-      <c r="A43" s="14"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="10"/>
-    </row>
-    <row r="44" ht="16.35" customHeight="1">
-      <c r="A44" s="14"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="10"/>
-    </row>
-    <row r="45" ht="16.35" customHeight="1">
-      <c r="A45" s="14"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="10"/>
-    </row>
-    <row r="46" ht="16.35" customHeight="1">
-      <c r="A46" s="14"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="10"/>
+      <c r="E40" s="10">
+        <v>10000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>